<commit_message>
Updates to yale faces demo
</commit_message>
<xml_diff>
--- a/Applications/YaleFaces/Step02_PreprocessDataset/Step02_IDs.xlsx
+++ b/Applications/YaleFaces/Step02_PreprocessDataset/Step02_IDs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MatlabAIML\Applications\YaleFaces\Step02_PreprocessDataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lum\GitHub\MatlabAIML\Applications\YaleFaces\Step02_PreprocessDataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AC2FFC-2790-4F32-98A4-93F800BFD8A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17030" yWindow="-18120" windowWidth="29040" windowHeight="18240"/>
+    <workbookView xWindow="17025" yWindow="-18120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step02A" sheetId="1" r:id="rId1"/>
@@ -20,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>^</t>
   </si>
@@ -47,54 +37,12 @@
     <t>File</t>
   </si>
   <si>
-    <t>flatDataFile</t>
-  </si>
-  <si>
     <t>TrainingAndTestDataScenario1.mat</t>
   </si>
   <si>
-    <t>numTrainingSamples</t>
-  </si>
-  <si>
-    <t>numTestSamples</t>
-  </si>
-  <si>
     <t>TrainingAndTestDataScenario2.mat</t>
   </si>
   <si>
-    <t>similar to TrainingAndTestDataScenario1 but randomly shuffle set</t>
-  </si>
-  <si>
-    <t>TrainingAndTestDataScenario3.mat</t>
-  </si>
-  <si>
-    <t>small set for testing</t>
-  </si>
-  <si>
-    <t>FlatDatasetScenario2.mat</t>
-  </si>
-  <si>
-    <t>TrainingAndTestDataScenario4.mat</t>
-  </si>
-  <si>
-    <t>FlatDatasetScenario3.mat</t>
-  </si>
-  <si>
-    <t>TrainingAndTestDataScenario5.mat</t>
-  </si>
-  <si>
-    <t>D values are all 0.1 and 0.9</t>
-  </si>
-  <si>
-    <t>D values are all 0.2 and 0.8</t>
-  </si>
-  <si>
-    <t>D values are all 0.0 and 1.0</t>
-  </si>
-  <si>
-    <t>CroppedDatasetScenario1.mat</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -102,12 +50,24 @@
   </si>
   <si>
     <t>no preprocessing</t>
+  </si>
+  <si>
+    <t>PreprocessedDatasetScenario2.mat</t>
+  </si>
+  <si>
+    <t>cropped to only face and center images</t>
+  </si>
+  <si>
+    <t>preprocessedDatasetFile</t>
+  </si>
+  <si>
+    <t>Use subject 14 and 15 as test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -473,29 +433,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -505,12 +465,20 @@
       <c r="H1" s="3"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -520,135 +488,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1796875" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>50000</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>50000</v>
-      </c>
-      <c r="D5">
-        <v>10000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>